<commit_message>
add significant documentation of SCCs
</commit_message>
<xml_diff>
--- a/_transportation/data-raw/epa/onroad_activity_data_SCC_descriptions.xlsx
+++ b/_transportation/data-raw/epa/onroad_activity_data_SCC_descriptions.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/godfrey_janice_epa_gov/Documents/Documents/SCC/Mobile/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cta\spreadsheets\pf7\WO 150.5 (2014v2)\onroad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F55B687A-20F2-4F51-A09F-6E15A22387DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="VMT" sheetId="1" r:id="rId1"/>
@@ -128,7 +127,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -439,24 +438,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -473,7 +472,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2201110200</v>
       </c>
@@ -490,7 +489,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2201110300</v>
       </c>
@@ -507,7 +506,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2201110400</v>
       </c>
@@ -524,7 +523,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2201110500</v>
       </c>
@@ -541,7 +540,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2201210200</v>
       </c>
@@ -558,7 +557,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2201210300</v>
       </c>
@@ -575,7 +574,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2201210400</v>
       </c>
@@ -592,7 +591,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2201210500</v>
       </c>
@@ -609,7 +608,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2201310200</v>
       </c>
@@ -626,7 +625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2201310300</v>
       </c>
@@ -643,7 +642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2201310400</v>
       </c>
@@ -660,7 +659,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2201310500</v>
       </c>
@@ -677,7 +676,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2201320200</v>
       </c>
@@ -694,7 +693,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2201320300</v>
       </c>
@@ -711,7 +710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2201320400</v>
       </c>
@@ -728,7 +727,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2201320500</v>
       </c>
@@ -745,7 +744,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2201410200</v>
       </c>
@@ -762,7 +761,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2201410300</v>
       </c>
@@ -779,7 +778,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2201410400</v>
       </c>
@@ -796,7 +795,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2201410500</v>
       </c>
@@ -813,7 +812,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2201420200</v>
       </c>
@@ -830,7 +829,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2201420300</v>
       </c>
@@ -847,7 +846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2201420400</v>
       </c>
@@ -864,7 +863,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2201420500</v>
       </c>
@@ -881,7 +880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2201430200</v>
       </c>
@@ -898,7 +897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2201430300</v>
       </c>
@@ -915,7 +914,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2201430400</v>
       </c>
@@ -932,7 +931,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2201430500</v>
       </c>
@@ -949,7 +948,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2201510200</v>
       </c>
@@ -966,7 +965,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2201510300</v>
       </c>
@@ -983,7 +982,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2201510400</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2201510500</v>
       </c>
@@ -1017,7 +1016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2201520200</v>
       </c>
@@ -1034,7 +1033,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2201520300</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2201520400</v>
       </c>
@@ -1068,7 +1067,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2201520500</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2201530200</v>
       </c>
@@ -1102,7 +1101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2201530300</v>
       </c>
@@ -1119,7 +1118,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2201530400</v>
       </c>
@@ -1136,7 +1135,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2201530500</v>
       </c>
@@ -1153,7 +1152,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2201540200</v>
       </c>
@@ -1170,7 +1169,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2201540300</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2201540400</v>
       </c>
@@ -1204,7 +1203,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2201540500</v>
       </c>
@@ -1221,7 +1220,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2201610200</v>
       </c>
@@ -1238,7 +1237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2201610300</v>
       </c>
@@ -1255,7 +1254,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2201610400</v>
       </c>
@@ -1272,7 +1271,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2201610500</v>
       </c>
@@ -1289,7 +1288,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2201620200</v>
       </c>
@@ -1306,7 +1305,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2201620300</v>
       </c>
@@ -1323,7 +1322,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2201620400</v>
       </c>
@@ -1340,7 +1339,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2201620500</v>
       </c>
@@ -1357,7 +1356,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2202110200</v>
       </c>
@@ -1374,7 +1373,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2202110300</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2202110400</v>
       </c>
@@ -1408,7 +1407,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2202110500</v>
       </c>
@@ -1425,7 +1424,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2202210200</v>
       </c>
@@ -1442,7 +1441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2202210300</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2202210400</v>
       </c>
@@ -1476,7 +1475,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2202210500</v>
       </c>
@@ -1493,7 +1492,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2202310200</v>
       </c>
@@ -1510,7 +1509,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2202310300</v>
       </c>
@@ -1527,7 +1526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2202310400</v>
       </c>
@@ -1544,7 +1543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2202310500</v>
       </c>
@@ -1561,7 +1560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2202320200</v>
       </c>
@@ -1578,7 +1577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2202320300</v>
       </c>
@@ -1595,7 +1594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2202320400</v>
       </c>
@@ -1612,7 +1611,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2202320500</v>
       </c>
@@ -1629,7 +1628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2202410200</v>
       </c>
@@ -1646,7 +1645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2202410300</v>
       </c>
@@ -1663,7 +1662,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2202410400</v>
       </c>
@@ -1680,7 +1679,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2202410500</v>
       </c>
@@ -1697,7 +1696,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2202420200</v>
       </c>
@@ -1714,7 +1713,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2202420300</v>
       </c>
@@ -1731,7 +1730,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2202420400</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2202420500</v>
       </c>
@@ -1765,7 +1764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2202430200</v>
       </c>
@@ -1782,7 +1781,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2202430300</v>
       </c>
@@ -1799,7 +1798,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2202430400</v>
       </c>
@@ -1816,7 +1815,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2202430500</v>
       </c>
@@ -1833,7 +1832,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2202510200</v>
       </c>
@@ -1850,7 +1849,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2202510300</v>
       </c>
@@ -1867,7 +1866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2202510400</v>
       </c>
@@ -1884,7 +1883,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2202510500</v>
       </c>
@@ -1901,7 +1900,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2202520200</v>
       </c>
@@ -1918,7 +1917,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2202520300</v>
       </c>
@@ -1935,7 +1934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2202520400</v>
       </c>
@@ -1952,7 +1951,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2202520500</v>
       </c>
@@ -1969,7 +1968,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2202530200</v>
       </c>
@@ -1986,7 +1985,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2202530300</v>
       </c>
@@ -2003,7 +2002,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2202530400</v>
       </c>
@@ -2020,7 +2019,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2202530500</v>
       </c>
@@ -2037,7 +2036,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2202540200</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2202540300</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2202540400</v>
       </c>
@@ -2088,7 +2087,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2202540500</v>
       </c>
@@ -2105,7 +2104,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2202610200</v>
       </c>
@@ -2122,7 +2121,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2202610300</v>
       </c>
@@ -2139,7 +2138,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2202610400</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2202610500</v>
       </c>
@@ -2173,7 +2172,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2202620200</v>
       </c>
@@ -2190,7 +2189,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2202620300</v>
       </c>
@@ -2207,7 +2206,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2202620400</v>
       </c>
@@ -2224,7 +2223,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2202620500</v>
       </c>
@@ -2241,7 +2240,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2203420200</v>
       </c>
@@ -2258,7 +2257,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2203420300</v>
       </c>
@@ -2275,7 +2274,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2203420400</v>
       </c>
@@ -2292,7 +2291,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>2203420500</v>
       </c>
@@ -2309,7 +2308,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>2205210200</v>
       </c>
@@ -2326,7 +2325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2205210300</v>
       </c>
@@ -2343,7 +2342,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>2205210400</v>
       </c>
@@ -2360,7 +2359,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>2205210500</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>2205310200</v>
       </c>
@@ -2394,7 +2393,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>2205310300</v>
       </c>
@@ -2411,7 +2410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>2205310400</v>
       </c>
@@ -2428,7 +2427,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>2205310500</v>
       </c>
@@ -2445,7 +2444,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>2205320200</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>2205320300</v>
       </c>
@@ -2479,7 +2478,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>2205320400</v>
       </c>
@@ -2496,7 +2495,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>2205320500</v>
       </c>
@@ -2513,7 +2512,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>2209210200</v>
       </c>
@@ -2530,7 +2529,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>2209210300</v>
       </c>
@@ -2547,7 +2546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>2209210400</v>
       </c>
@@ -2564,7 +2563,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>2209210500</v>
       </c>
@@ -2581,7 +2580,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>2209310200</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>2209310300</v>
       </c>
@@ -2615,7 +2614,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>2209310400</v>
       </c>
@@ -2632,7 +2631,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>2209310500</v>
       </c>
@@ -2649,7 +2648,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>2209320200</v>
       </c>
@@ -2666,7 +2665,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>2209320300</v>
       </c>
@@ -2683,7 +2682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>2209320400</v>
       </c>
@@ -2700,7 +2699,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>2209320500</v>
       </c>
@@ -2718,7 +2717,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G165">
+  <sortState ref="A2:G165">
     <sortCondition ref="A2:A165"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2726,24 +2725,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -2760,7 +2759,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2201110100</v>
       </c>
@@ -2777,7 +2776,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2201210100</v>
       </c>
@@ -2794,7 +2793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2201310100</v>
       </c>
@@ -2811,7 +2810,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2201320100</v>
       </c>
@@ -2828,7 +2827,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2201410100</v>
       </c>
@@ -2845,7 +2844,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2201420100</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2201430100</v>
       </c>
@@ -2879,7 +2878,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2201510100</v>
       </c>
@@ -2896,7 +2895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2201520100</v>
       </c>
@@ -2913,7 +2912,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2201530100</v>
       </c>
@@ -2930,7 +2929,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2201540100</v>
       </c>
@@ -2947,7 +2946,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2201610100</v>
       </c>
@@ -2964,7 +2963,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2201620100</v>
       </c>
@@ -2981,7 +2980,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2202110100</v>
       </c>
@@ -2998,7 +2997,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2202210100</v>
       </c>
@@ -3015,7 +3014,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2202310100</v>
       </c>
@@ -3032,7 +3031,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2202320100</v>
       </c>
@@ -3049,7 +3048,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2202410100</v>
       </c>
@@ -3066,7 +3065,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2202420100</v>
       </c>
@@ -3083,7 +3082,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2202430100</v>
       </c>
@@ -3100,7 +3099,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2202510100</v>
       </c>
@@ -3117,7 +3116,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2202520100</v>
       </c>
@@ -3134,7 +3133,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2202530100</v>
       </c>
@@ -3151,7 +3150,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2202540100</v>
       </c>
@@ -3168,7 +3167,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2202610100</v>
       </c>
@@ -3185,7 +3184,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2202620100</v>
       </c>
@@ -3202,7 +3201,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2203420100</v>
       </c>
@@ -3219,7 +3218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2205210100</v>
       </c>
@@ -3236,7 +3235,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2205310100</v>
       </c>
@@ -3253,7 +3252,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2205320100</v>
       </c>
@@ -3270,7 +3269,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2209210100</v>
       </c>
@@ -3287,7 +3286,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2209310100</v>
       </c>
@@ -3304,7 +3303,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2209320100</v>
       </c>
@@ -3327,7 +3326,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3335,16 +3334,16 @@
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -3361,7 +3360,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2202620153</v>
       </c>
@@ -3378,7 +3377,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2202620191</v>
       </c>

</xml_diff>